<commit_message>
code for top rated r file
</commit_message>
<xml_diff>
--- a/sub_pro_24_top_rated_online/top_rated_online_feb_2025.xlsx
+++ b/sub_pro_24_top_rated_online/top_rated_online_feb_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\afro_dataviz\sub_pro_24_top_rated_online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883B94D0-A0CE-4B3A-BD86-76A056EEA652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AAA50B-6E7A-4ECC-AF8F-D7E615A42E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3237B7C4-AF31-4C7B-B7C7-6A62318D4F82}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>COG</t>
   </si>
   <si>
-    <t>CONGO, THE DEMOCRATIC REPUBLIC OF THE</t>
-  </si>
-  <si>
     <t>CD</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
     <t>LBR</t>
   </si>
   <si>
-    <t>LIBYAN ARAB JAMAHIRIYA</t>
-  </si>
-  <si>
     <t>LY</t>
   </si>
   <si>
@@ -483,9 +477,6 @@
     <t>SWZ</t>
   </si>
   <si>
-    <t>TANZANIA, UNITED REPUBLIC OF</t>
-  </si>
-  <si>
     <t>TZ</t>
   </si>
   <si>
@@ -787,6 +778,15 @@
   </si>
   <si>
     <t>Joina City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIBYAN </t>
+  </si>
+  <si>
+    <t>CONGO, DR</t>
+  </si>
+  <si>
+    <t>TANZANIA</t>
   </si>
 </sst>
 </file>
@@ -1154,13 +1154,13 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.90625" customWidth="1"/>
     <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
@@ -1181,22 +1181,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1210,10 +1210,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F2" s="2">
         <v>7700</v>
@@ -1233,10 +1233,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2">
         <v>4500</v>
@@ -1256,10 +1256,10 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F4" s="2">
         <v>7800</v>
@@ -1279,10 +1279,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F5" s="2">
         <v>4400</v>
@@ -1302,10 +1302,10 @@
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F6" s="2">
         <v>5000</v>
@@ -1325,10 +1325,10 @@
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F7" s="2">
         <v>390</v>
@@ -1348,10 +1348,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F8" s="2">
         <v>7000</v>
@@ -1371,10 +1371,10 @@
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F9" s="2">
         <v>6900</v>
@@ -1394,10 +1394,10 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F10" s="2">
         <v>352</v>
@@ -1417,10 +1417,10 @@
         <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F11" s="2">
         <v>555</v>
@@ -1440,10 +1440,10 @@
         <v>35</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F12" s="2">
         <v>397</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>36</v>
@@ -1463,10 +1463,10 @@
         <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F13" s="2">
         <v>480</v>
@@ -1477,19 +1477,19 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F14" s="2">
         <v>4800</v>
@@ -1500,19 +1500,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F15" s="2">
         <v>11000</v>
@@ -1523,19 +1523,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F16" s="2">
         <v>2700</v>
@@ -1546,19 +1546,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F17" s="2">
         <v>134700</v>
@@ -1569,19 +1569,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F18" s="2">
         <v>302</v>
@@ -1592,19 +1592,19 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F19" s="2">
         <v>299</v>
@@ -1615,19 +1615,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F20" s="2">
         <v>5800</v>
@@ -1638,19 +1638,19 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F21" s="2">
         <v>3500</v>
@@ -1661,19 +1661,19 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F22" s="2">
         <v>1200</v>
@@ -1684,19 +1684,19 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F23" s="2">
         <v>32400</v>
@@ -1707,19 +1707,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F24" s="2">
         <v>705</v>
@@ -1730,19 +1730,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F25" s="2">
         <v>797</v>
@@ -1753,19 +1753,19 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F26" s="2">
         <v>28100</v>
@@ -1776,19 +1776,19 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F27" s="2">
         <v>991</v>
@@ -1799,19 +1799,19 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F28" s="2">
         <v>499</v>
@@ -1822,19 +1822,19 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F29" s="2">
         <v>12600</v>
@@ -1845,19 +1845,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F30" s="2">
         <v>1200</v>
@@ -1868,19 +1868,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F31" s="2">
         <v>3700</v>
@@ -1891,19 +1891,19 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F32" s="2">
         <v>726</v>
@@ -1914,19 +1914,19 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F33" s="2">
         <v>1700</v>
@@ -1937,19 +1937,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F34" s="2">
         <v>17400</v>
@@ -1960,42 +1960,42 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F36" s="2">
         <v>49200</v>
@@ -2006,19 +2006,19 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F37" s="2">
         <v>5100</v>
@@ -2029,19 +2029,19 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F38" s="2">
         <v>8500</v>
@@ -2052,19 +2052,19 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F39" s="2">
         <v>4400</v>
@@ -2075,19 +2075,19 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F40" s="2">
         <v>45500</v>
@@ -2098,42 +2098,42 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F42" s="2">
         <v>4300</v>
@@ -2144,19 +2144,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F43" s="2">
         <v>1300</v>
@@ -2167,19 +2167,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F44" s="2">
         <v>8600</v>
@@ -2190,19 +2190,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F45" s="2">
         <v>3100</v>
@@ -2213,19 +2213,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F46" s="2">
         <v>506</v>
@@ -2236,19 +2236,19 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F47" s="2">
         <v>916</v>
@@ -2259,19 +2259,19 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F48" s="2">
         <v>102200</v>
@@ -2282,19 +2282,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>145</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F49" s="2">
         <v>467</v>
@@ -2305,19 +2305,19 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F50" s="2">
         <v>24200</v>
@@ -2328,19 +2328,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F51" s="2">
         <v>1000</v>
@@ -2351,19 +2351,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>152</v>
+        <v>253</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F52" s="2">
         <v>18600</v>
@@ -2374,19 +2374,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F53" s="2">
         <v>5500</v>
@@ -2397,19 +2397,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F54" s="2">
         <v>9000</v>
@@ -2420,19 +2420,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F55" s="2">
         <v>9600</v>
@@ -2443,19 +2443,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F56" s="2">
         <v>92</v>
@@ -2466,19 +2466,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F57" s="2">
         <v>12900</v>
@@ -2489,19 +2489,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F58" s="2">
         <v>11300</v>

</xml_diff>